<commit_message>
src: correcciones de carga masiva y testeo funcionando
</commit_message>
<xml_diff>
--- a/src/resources/TestCargaMasivaColaboraciones.xlsx
+++ b/src/resources/TestCargaMasivaColaboraciones.xlsx
@@ -8,13 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Rocio\Documents\UTN\DDS\2024-tpa-mi-no-grupo-08\src\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F1E1EEF-DF30-4CEB-A97F-14A27B3227CA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2BE1252-3685-4BAD-8026-098B18711DB0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5316" yWindow="1488" windowWidth="17280" windowHeight="8964" tabRatio="489" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Hoja1!$B$1:$B$20</definedName>
+  </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -25,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="29">
   <si>
     <t>Tipo Doc</t>
   </si>
@@ -42,24 +45,12 @@
     <t>Mail</t>
   </si>
   <si>
-    <t>Fecha de colaboración</t>
-  </si>
-  <si>
-    <t>Forma de colaboración</t>
-  </si>
-  <si>
     <t>Cantidad</t>
   </si>
   <si>
     <t>DNI</t>
   </si>
   <si>
-    <t>Rocío</t>
-  </si>
-  <si>
-    <t>Ochoa Charlín</t>
-  </si>
-  <si>
     <t>rochoacharlin@frba.utn.edu.ar</t>
   </si>
   <si>
@@ -106,6 +97,24 @@
   </si>
   <si>
     <t>ENTREGA_TARJETAS</t>
+  </si>
+  <si>
+    <t>Fecha de colaboracion</t>
+  </si>
+  <si>
+    <t>Forma de colaboracion</t>
+  </si>
+  <si>
+    <t>Rocio</t>
+  </si>
+  <si>
+    <t>Ochoa Charlin</t>
+  </si>
+  <si>
+    <t>Teal 2</t>
+  </si>
+  <si>
+    <t>Music2</t>
   </si>
 </sst>
 </file>
@@ -115,7 +124,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="dd/mm/yyyy;@"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -127,14 +136,6 @@
       <u/>
       <sz val="11"/>
       <color theme="10"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -166,7 +167,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
@@ -448,10 +449,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J20"/>
+  <dimension ref="A1:H20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J10" sqref="J10"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -464,7 +465,7 @@
     <col min="7" max="7" width="23.77734375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -481,392 +482,391 @@
         <v>4</v>
       </c>
       <c r="F1" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="G1" t="s">
+        <v>24</v>
+      </c>
+      <c r="H1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B2" s="2">
         <v>44125678</v>
       </c>
       <c r="C2" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="D2" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="F2" s="3">
         <v>45437</v>
       </c>
       <c r="G2" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="H2">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B3" s="2">
         <v>44125678</v>
       </c>
       <c r="C3" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="D3" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="F3" s="3">
         <v>45438</v>
       </c>
       <c r="G3" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="H3">
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B4" s="2">
         <v>43225217</v>
       </c>
       <c r="C4" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="F4" s="3">
         <v>45439</v>
       </c>
       <c r="G4" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="H4">
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B5" s="2">
         <v>43225217</v>
       </c>
       <c r="C5" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="F5" s="3">
         <v>45440</v>
       </c>
       <c r="G5" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="H5">
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B6" s="2">
         <v>43225217</v>
       </c>
       <c r="C6" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="F6" s="3">
         <v>45441</v>
       </c>
       <c r="G6" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="H6">
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B7" s="2">
         <v>44125678</v>
       </c>
       <c r="C7" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="D7" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="F7" s="3">
         <v>45442</v>
       </c>
       <c r="G7" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="H7">
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B8" s="2">
         <v>45478895</v>
       </c>
       <c r="C8" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="D8" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="F8" s="3">
         <v>45443</v>
       </c>
       <c r="G8" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="H8">
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B9" s="2">
         <v>45478895</v>
       </c>
       <c r="C9" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="D9" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="F9" s="3">
         <v>45444</v>
       </c>
       <c r="G9" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="H9">
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B10" s="2">
         <v>41235976</v>
       </c>
       <c r="C10" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="D10" t="s">
+        <v>14</v>
+      </c>
+      <c r="E10" s="1" t="s">
         <v>18</v>
-      </c>
-      <c r="E10" s="1" t="s">
-        <v>22</v>
       </c>
       <c r="F10" s="3">
         <v>45445</v>
       </c>
       <c r="G10" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="H10">
         <v>2</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B11" s="2">
         <v>41365749</v>
       </c>
       <c r="C11" t="s">
-        <v>17</v>
+        <v>27</v>
       </c>
       <c r="D11" t="s">
+        <v>28</v>
+      </c>
+      <c r="E11" s="1" t="s">
         <v>18</v>
-      </c>
-      <c r="E11" s="1" t="s">
-        <v>22</v>
       </c>
       <c r="F11" s="3">
         <v>45446</v>
       </c>
       <c r="G11" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="H11">
         <v>3</v>
       </c>
-      <c r="J11" s="4"/>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B12" s="2">
         <v>44125678</v>
       </c>
       <c r="C12" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="D12" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="F12" s="3">
         <v>45447</v>
       </c>
       <c r="G12" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="H12">
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B13" s="2">
         <v>44651389</v>
       </c>
-      <c r="C13" t="s">
-        <v>9</v>
+      <c r="C13" s="4" t="s">
+        <v>25</v>
       </c>
       <c r="D13" t="s">
-        <v>10</v>
+        <v>26</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="F13" s="3">
         <v>45448</v>
       </c>
       <c r="G13" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="H13">
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B14" s="2">
         <v>44651389</v>
       </c>
       <c r="C14" t="s">
-        <v>9</v>
+        <v>25</v>
       </c>
       <c r="D14" t="s">
-        <v>10</v>
+        <v>26</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="F14" s="3">
         <v>45449</v>
       </c>
       <c r="G14" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="H14">
         <v>2</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B15" s="2">
         <v>44651389</v>
       </c>
       <c r="C15" t="s">
-        <v>9</v>
+        <v>25</v>
       </c>
       <c r="D15" t="s">
-        <v>10</v>
+        <v>26</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="F15" s="3">
         <v>45450</v>
       </c>
       <c r="G15" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="H15">
         <v>3</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B16" s="2">
         <v>44651389</v>
       </c>
       <c r="C16" t="s">
-        <v>9</v>
+        <v>25</v>
       </c>
       <c r="D16" t="s">
-        <v>10</v>
+        <v>26</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="F16" s="3">
         <v>45451</v>
       </c>
       <c r="G16" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="H16">
         <v>4</v>
@@ -874,25 +874,25 @@
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B17" s="2">
         <v>44651389</v>
       </c>
       <c r="C17" t="s">
-        <v>9</v>
+        <v>25</v>
       </c>
       <c r="D17" t="s">
-        <v>10</v>
+        <v>26</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="F17" s="3">
         <v>45452</v>
       </c>
       <c r="G17" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="H17">
         <v>5</v>
@@ -900,25 +900,25 @@
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B18" s="2">
         <v>44651389</v>
       </c>
       <c r="C18" t="s">
-        <v>9</v>
+        <v>25</v>
       </c>
       <c r="D18" t="s">
-        <v>10</v>
+        <v>26</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="F18" s="3">
         <v>45453</v>
       </c>
       <c r="G18" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="H18">
         <v>10</v>
@@ -926,25 +926,25 @@
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B19" s="2">
         <v>44651389</v>
       </c>
       <c r="C19" t="s">
-        <v>9</v>
+        <v>25</v>
       </c>
       <c r="D19" t="s">
-        <v>10</v>
+        <v>26</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="F19" s="3">
         <v>45454</v>
       </c>
       <c r="G19" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="H19">
         <v>7</v>
@@ -952,25 +952,25 @@
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B20" s="2">
         <v>44651389</v>
       </c>
       <c r="C20" t="s">
-        <v>9</v>
+        <v>25</v>
       </c>
       <c r="D20" t="s">
-        <v>10</v>
+        <v>26</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="F20" s="3">
         <v>45455</v>
       </c>
       <c r="G20" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="H20">
         <v>8</v>
@@ -999,5 +999,6 @@
     <hyperlink ref="E11" r:id="rId19" xr:uid="{12E593C9-27AC-4392-8CB1-541534BB3C63}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId20"/>
 </worksheet>
 </file>
</xml_diff>